<commit_message>
Excel viewer and Uploader (will debug later)
</commit_message>
<xml_diff>
--- a/public/Downloads/Accounts.xlsx
+++ b/public/Downloads/Accounts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>2023-06-12T17:27:12.000000Z</t>
+  </si>
+  <si>
+    <t>Mazeu</t>
+  </si>
+  <si>
+    <t>maze@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-06-12T21:00:44.000000Z</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +459,23 @@
       </c>
       <c r="F3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>